<commit_message>
Cleanup and new Ship Data Bottle Sample Summaries for Pioneer.
</commit_message>
<xml_diff>
--- a/Ship_data/Pioneer/Pioneer-06_AR-04_2016-05-12/Pioneer-06_AR04_Discrete_Summary_2019-07-15_ver_1-02_.xlsx
+++ b/Ship_data/Pioneer/Pioneer-06_AR-04_2016-05-12/Pioneer-06_AR04_Discrete_Summary_2019-07-15_ver_1-02_.xlsx
@@ -1201,87 +1201,87 @@
   </sheetPr>
   <dimension ref="A1:BZ119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AN1" activeCellId="0" sqref="AN1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CJ15" activeCellId="0" sqref="CJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="23.85"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="27.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="25.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="40.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="40.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="39.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="21.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="0" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="21.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="30.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="26.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="35.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="23.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="23.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="27.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="22.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="32.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="30.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="22.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="22.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="21.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="31.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="29.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="24.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="0" width="14.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="27.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="27.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="24.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="20.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="16.35"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="20" style="0" width="27.49"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="21" min="21" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="25" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="0" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="23.3"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="25.61"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="40.6"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="35" min="35" style="0" width="40.16"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="36" min="36" style="0" width="39.51"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="37" style="0" width="21.75"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="39" min="38" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="40" min="40" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="41" min="41" style="0" width="21.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="42" min="42" style="0" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="43" min="43" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="44" min="44" style="0" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="45" min="45" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="46" min="46" style="0" width="26.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="47" min="47" style="0" width="35.53"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="48" min="48" style="0" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="49" min="49" style="0" width="24.06"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="50" min="50" style="0" width="23.74"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="51" min="51" style="0" width="23.19"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="52" min="52" style="0" width="27.93"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="53" min="53" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="54" min="54" style="0" width="32.11"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="55" min="55" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="56" min="56" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="57" min="57" style="0" width="30.35"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="58" min="58" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="59" min="59" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="60" min="60" style="0" width="22.19"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="61" min="61" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="62" min="62" style="0" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="63" min="63" style="0" width="31.56"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="64" min="64" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="65" min="65" style="0" width="24.06"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="66" min="66" style="0" width="29.25"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="67" min="67" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="68" min="68" style="0" width="30.02"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="69" min="69" style="0" width="24.39"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="70" min="70" style="0" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="71" min="71" style="0" width="14.26"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="72" min="72" style="0" width="27.27"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="73" min="73" style="0" width="27.04"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="74" min="74" style="0" width="24.95"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="75" min="75" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="76" min="76" style="0" width="20.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="18.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="79" style="0" width="9.14"/>

</xml_diff>